<commit_message>
working model 50 trials
</commit_message>
<xml_diff>
--- a/data/raw-data/2022-student-research-case-study-football-soccer-data.xlsx
+++ b/data/raw-data/2022-student-research-case-study-football-soccer-data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77131FA-DDAB-46C1-9247-991989B3EC69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF07E71-8F7B-4CF2-ACBB-503DF2582347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -431,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -483,6 +483,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,8 +716,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5297952" y="113714"/>
-          <a:ext cx="1020347" cy="542925"/>
+          <a:off x="5305572" y="113714"/>
+          <a:ext cx="1014632" cy="548640"/>
           <a:chOff x="3337560" y="82501"/>
           <a:chExt cx="1016537" cy="549519"/>
         </a:xfrm>
@@ -836,8 +837,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="257175" y="0"/>
-          <a:ext cx="1051266" cy="588792"/>
+          <a:off x="259080" y="0"/>
+          <a:ext cx="1055076" cy="592602"/>
           <a:chOff x="1337018" y="168519"/>
           <a:chExt cx="1046137" cy="591576"/>
         </a:xfrm>
@@ -965,8 +966,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="283845" y="125730"/>
-          <a:ext cx="1056981" cy="590697"/>
+          <a:off x="287655" y="123825"/>
+          <a:ext cx="1051266" cy="594507"/>
           <a:chOff x="1337018" y="168519"/>
           <a:chExt cx="1046137" cy="591576"/>
         </a:xfrm>
@@ -1089,8 +1090,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5955030" y="112395"/>
-          <a:ext cx="1005107" cy="542925"/>
+          <a:off x="5953125" y="112395"/>
+          <a:ext cx="1008917" cy="548640"/>
           <a:chOff x="3337560" y="82501"/>
           <a:chExt cx="1016537" cy="549519"/>
         </a:xfrm>
@@ -1215,8 +1216,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="281940" y="129540"/>
-          <a:ext cx="1062696" cy="583077"/>
+          <a:off x="285750" y="125730"/>
+          <a:ext cx="1056981" cy="596412"/>
           <a:chOff x="1337018" y="168519"/>
           <a:chExt cx="1046137" cy="591576"/>
         </a:xfrm>
@@ -1339,8 +1340,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5958840" y="62865"/>
-          <a:ext cx="1003202" cy="542925"/>
+          <a:off x="5955030" y="64770"/>
+          <a:ext cx="1008917" cy="548640"/>
           <a:chOff x="3337560" y="82501"/>
           <a:chExt cx="1016537" cy="549519"/>
         </a:xfrm>
@@ -1465,8 +1466,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="278130" y="133350"/>
-          <a:ext cx="1062696" cy="583077"/>
+          <a:off x="283845" y="129540"/>
+          <a:ext cx="1062696" cy="588792"/>
           <a:chOff x="1337018" y="168519"/>
           <a:chExt cx="1046137" cy="591576"/>
         </a:xfrm>
@@ -1589,8 +1590,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3238500" y="28575"/>
-          <a:ext cx="1012727" cy="542925"/>
+          <a:off x="3238500" y="30480"/>
+          <a:ext cx="1008917" cy="548640"/>
           <a:chOff x="3337560" y="82501"/>
           <a:chExt cx="1016537" cy="549519"/>
         </a:xfrm>
@@ -1715,8 +1716,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="274320" y="129540"/>
-          <a:ext cx="1070316" cy="583077"/>
+          <a:off x="280035" y="133350"/>
+          <a:ext cx="1062696" cy="588792"/>
           <a:chOff x="1337018" y="168519"/>
           <a:chExt cx="1046137" cy="591576"/>
         </a:xfrm>
@@ -1839,8 +1840,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4838700" y="47625"/>
-          <a:ext cx="1012727" cy="542925"/>
+          <a:off x="4838700" y="45720"/>
+          <a:ext cx="1008917" cy="548640"/>
           <a:chOff x="3337560" y="82501"/>
           <a:chExt cx="1016537" cy="549519"/>
         </a:xfrm>
@@ -2205,7 +2206,7 @@
   </sheetPr>
   <dimension ref="B7:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -5489,10 +5490,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B7:G37"/>
+  <dimension ref="B7:H37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5503,27 +5504,27 @@
     <col min="7" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D12" s="22"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:7" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
@@ -5543,7 +5544,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>8</v>
       </c>
@@ -5562,8 +5563,12 @@
       <c r="G14" s="24">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="25">
+        <f>SUM(C14:G14)</f>
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
@@ -5582,8 +5587,12 @@
       <c r="G15" s="24">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="25">
+        <f t="shared" ref="H15:H34" si="0">SUM(C15:G15)</f>
+        <v>75.900000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
@@ -5602,8 +5611,12 @@
       <c r="G16" s="24">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="25">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000025</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
@@ -5622,8 +5635,12 @@
       <c r="G17" s="24">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>1</v>
       </c>
@@ -5642,8 +5659,12 @@
       <c r="G18" s="24">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="25">
+        <f t="shared" si="0"/>
+        <v>89.600000000000009</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>22</v>
       </c>
@@ -5662,8 +5683,12 @@
       <c r="G19" s="24">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="25">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
@@ -5682,8 +5707,12 @@
       <c r="G20" s="24">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="25">
+        <f t="shared" si="0"/>
+        <v>87.100000000000009</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>4</v>
       </c>
@@ -5702,8 +5731,12 @@
       <c r="G21" s="24" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="25">
+        <f t="shared" si="0"/>
+        <v>7.8999999999999986</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>2</v>
       </c>
@@ -5722,8 +5755,12 @@
       <c r="G22" s="24">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="25">
+        <f t="shared" si="0"/>
+        <v>9.3999999999999986</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>10</v>
       </c>
@@ -5742,8 +5779,12 @@
       <c r="G23" s="24">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="25">
+        <f t="shared" si="0"/>
+        <v>91.7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>23</v>
       </c>
@@ -5762,8 +5803,12 @@
       <c r="G24" s="24">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="25">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>13</v>
       </c>
@@ -5782,8 +5827,12 @@
       <c r="G25" s="24">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="25">
+        <f t="shared" si="0"/>
+        <v>93.2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
         <v>0</v>
       </c>
@@ -5802,8 +5851,12 @@
       <c r="G26" s="24">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="25">
+        <f t="shared" si="0"/>
+        <v>247.99999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>24</v>
       </c>
@@ -5822,8 +5875,12 @@
       <c r="G27" s="24">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="25">
+        <f t="shared" si="0"/>
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
         <v>5</v>
       </c>
@@ -5842,8 +5899,12 @@
       <c r="G28" s="24">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="25">
+        <f t="shared" si="0"/>
+        <v>140.79999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
         <v>7</v>
       </c>
@@ -5862,8 +5923,12 @@
       <c r="G29" s="24">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H29" s="25">
+        <f t="shared" si="0"/>
+        <v>76.400000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
         <v>14</v>
       </c>
@@ -5882,8 +5947,12 @@
       <c r="G30" s="24">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="25">
+        <f t="shared" si="0"/>
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
         <v>3</v>
       </c>
@@ -5902,8 +5971,12 @@
       <c r="G31" s="24">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="25">
+        <f t="shared" si="0"/>
+        <v>102.89999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
         <v>6</v>
       </c>
@@ -5922,8 +5995,12 @@
       <c r="G32" s="24">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H32" s="25">
+        <f t="shared" si="0"/>
+        <v>251.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
         <v>9</v>
       </c>
@@ -5942,8 +6019,12 @@
       <c r="G33" s="24">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="25">
+        <f t="shared" si="0"/>
+        <v>4.6999999999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
         <v>12</v>
       </c>
@@ -5962,8 +6043,12 @@
       <c r="G34" s="24">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="25">
+        <f t="shared" si="0"/>
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G37" s="8" t="s">
         <v>16</v>
       </c>

</xml_diff>